<commit_message>
Organised stuff, changed forest
</commit_message>
<xml_diff>
--- a/Documents/Prototype values.xlsx
+++ b/Documents/Prototype values.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Root</t>
   </si>
@@ -34,6 +34,57 @@
   </si>
   <si>
     <t>Sell</t>
+  </si>
+  <si>
+    <t>Profit x1</t>
+  </si>
+  <si>
+    <t>Profit x10</t>
+  </si>
+  <si>
+    <t>*Assuming linear progression, unlimited time, no plant deaths/premature harvests, and unlimited garden space</t>
+  </si>
+  <si>
+    <t>Profit x5</t>
+  </si>
+  <si>
+    <t>Profit x15</t>
+  </si>
+  <si>
+    <t>Profit x20</t>
+  </si>
+  <si>
+    <t>Profit x30</t>
+  </si>
+  <si>
+    <t>Profit x40</t>
+  </si>
+  <si>
+    <t>Profit x50</t>
+  </si>
+  <si>
+    <t>Profit x60</t>
+  </si>
+  <si>
+    <t>Profit x70</t>
+  </si>
+  <si>
+    <t>Profit x80</t>
+  </si>
+  <si>
+    <t>Profit x90</t>
+  </si>
+  <si>
+    <t>Profit x100</t>
+  </si>
+  <si>
+    <t>Profit x1000</t>
+  </si>
+  <si>
+    <t>Net loss</t>
+  </si>
+  <si>
+    <t>Net gain</t>
   </si>
 </sst>
 </file>
@@ -49,12 +100,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,8 +138,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,51 +423,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D4"/>
+  <dimension ref="B2:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>45</v>
-      </c>
-      <c r="D3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="2">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="C4" s="3">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <f>C4-C3</f>
+        <v>4</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ref="D6:E6" si="0">D4-D3</f>
+        <v>-11</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <f>(C4*5)-(C3*5)</f>
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <f>(D4*5)-(D3*1)</f>
+        <v>29</v>
+      </c>
+      <c r="E7" s="3">
+        <f>(E4*5)-E3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <f>(C4*10)-(C3*10)</f>
+        <v>40</v>
+      </c>
+      <c r="D8" s="3">
+        <f>(D4*10)-(D3*2)</f>
+        <v>58</v>
+      </c>
+      <c r="E8" s="3">
+        <f>(E4*10)-E3</f>
+        <v>55</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(C4*15)-(C3*15)</f>
+        <v>60</v>
+      </c>
+      <c r="D9" s="3">
+        <f>(D4*15)-(D3*3)</f>
+        <v>87</v>
+      </c>
+      <c r="E9" s="3">
+        <f>(E4*15)-E3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(C4*20)-(C3*20)</f>
+        <v>80</v>
+      </c>
+      <c r="D10" s="3">
+        <f>(D4*20)-(D3*4)</f>
+        <v>116</v>
+      </c>
+      <c r="E10" s="3">
+        <f>(E4*20)-E3</f>
+        <v>145</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(C4*30)-(C3*30)</f>
+        <v>120</v>
+      </c>
+      <c r="D11" s="3">
+        <f>(D4*30)-(D3*6)</f>
+        <v>174</v>
+      </c>
+      <c r="E11" s="3">
+        <f>(E4*30)-E3</f>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3">
+        <f>(C4*40)-(C3*40)</f>
+        <v>160</v>
+      </c>
+      <c r="D12" s="3">
+        <f>(D4*40)-(D3*8)</f>
+        <v>232</v>
+      </c>
+      <c r="E12" s="3">
+        <f>(E4*40)-E3</f>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3">
+        <f>(C4*50)-(C3*50)</f>
+        <v>200</v>
+      </c>
+      <c r="D13" s="3">
+        <f>(D4*50)-(D3*10)</f>
+        <v>290</v>
+      </c>
+      <c r="E13" s="3">
+        <f>(E4*50)-E3</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3">
+        <f>(C4*60)-(C3*60)</f>
+        <v>240</v>
+      </c>
+      <c r="D14" s="3">
+        <f>(D4*60)-(D3*12)</f>
+        <v>348</v>
+      </c>
+      <c r="E14" s="3">
+        <f>(E4*60)-E3</f>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
+      <c r="C15" s="3">
+        <f>(C4*70)-(C3*70)</f>
+        <v>280</v>
+      </c>
+      <c r="D15" s="3">
+        <f>(D4*70)-(D3*14)</f>
+        <v>406</v>
+      </c>
+      <c r="E15" s="3">
+        <f>(E4*70)-E3</f>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3">
+        <f>(C4*80)-(C3*80)</f>
+        <v>320</v>
+      </c>
+      <c r="D16" s="3">
+        <f>(D4*80)-(D3*16)</f>
+        <v>464</v>
+      </c>
+      <c r="E16" s="3">
+        <f>(E4*80)-E3</f>
+        <v>685</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3">
+        <f>(C4*90)-(C3*90)</f>
+        <v>360</v>
+      </c>
+      <c r="D17" s="3">
+        <f>(D4*90)-(D3*18)</f>
+        <v>522</v>
+      </c>
+      <c r="E17" s="3">
+        <f>(E4*90)-E3</f>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <f>(C4*100)-(C3*100)</f>
+        <v>400</v>
+      </c>
+      <c r="D18" s="3">
+        <f>(D4*100)-(D3*20)</f>
+        <v>580</v>
+      </c>
+      <c r="E18" s="3">
+        <f>(E4*100)-E3</f>
+        <v>865</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="3">
+        <f>(C4*1000)-(C3*1000)</f>
+        <v>4000</v>
+      </c>
+      <c r="D19" s="3">
+        <f>(D4*1000)-(D3*200)</f>
+        <v>5800</v>
+      </c>
+      <c r="E19" s="3">
+        <f>(E4*1000)-E3</f>
+        <v>8965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>